<commit_message>
Added non protected excel to read data
</commit_message>
<xml_diff>
--- a/input/Data/TumOnline/Read15S.xlsx
+++ b/input/Data/TumOnline/Read15S.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11250"/>
   </bookViews>
   <sheets>
-    <sheet name="Conflicts" sheetId="2" r:id="rId1"/>
+    <sheet name="Students" sheetId="3" r:id="rId1"/>
+    <sheet name="Conflicts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,11 +66,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -355,10 +353,4184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle9"/>
+  <dimension ref="A1:A831"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A799" workbookViewId="0">
+      <selection activeCell="D828" sqref="D828"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A398" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A399" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A400" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A401" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A402" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A403" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A404" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A405" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A406" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A407" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A408" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A409" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A410" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A411" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A412" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A413" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A414" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A415" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A416" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A417" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A418" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A419" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A420" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A421" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A422" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A423" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A424" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A425" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A426" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A427" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A428" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A429" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A430" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A431" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A432" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A433" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A434" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A435" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A436" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A437" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A438" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A439" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A440" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A441" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A442" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A443" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A444" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A445" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A446" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A447" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A448" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A449" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A450" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A451" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A452" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A453" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A454" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A455" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A456" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A457" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A458" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A459" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A460" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A461" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A462" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A463" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A464" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A465" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A466" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A467" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A468" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A469" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A470" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A471" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A472" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A473" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A474" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A475" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A476" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A477" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A478" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A479" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A480" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A481" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A482" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A483" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A484" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A485" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A486" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A487" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A488" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A489" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A490" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A491" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A492" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A493" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A494" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A495" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A496" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A497" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A498" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A499" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A500" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A501" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A502" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A503" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A504" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A505" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A506" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A507" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A508" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A509" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A510" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A511" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A512" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A513" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A514" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A515" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A516" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A517" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A518" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A519" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A520" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A521" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A522" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A523" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A524" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A525" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A526" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A527" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A528" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A529" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A530" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A531" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A532" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A533" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A534" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A535" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A536" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A537" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A538" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A539" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A540" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A541" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A542" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A543" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A544" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A545" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A546" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A547" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A548" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A549" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A550" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A551" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A552" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A553" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A554" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A555" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A556" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A557" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A558" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A559" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A560" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A561" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A562" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A563" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A564" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A565" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A566" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A567" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A568" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A569" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A570" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A571" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A572" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A573" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A574" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A575" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A576" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A577" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A578" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A579" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A580" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A581" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A582" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A583" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A584" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A585" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A586" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A587" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A588" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A589" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A590" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A591" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A592" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A593" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A594" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A595" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A596" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A597" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A598" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A599" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A600" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A601" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A602" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A603" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A604" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A605" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A606" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A607" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A608" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A609" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A610" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A611" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A612" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A613" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A614" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A615" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A616" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A617" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A618" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A619" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A620" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A621" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A622" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A623" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A624" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A625" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A626" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A627" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A628" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A629" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A630" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A631" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A632" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A633" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A634" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A635" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A636" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A637" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A638" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A639" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A640" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A641" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A642" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A643" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A644" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A645" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A646" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A647" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A648" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A649" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A650" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A651" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A652" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A653" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A654" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A655" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A656" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A657" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A658" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A659" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A660" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A661" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A662" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A663" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A664" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A665" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A666" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A667" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A668" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A669" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A670" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A671" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A672" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A673" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A674" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A675" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A676" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A677" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A678" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A679" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A680" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A681" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A682" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A683" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A684" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A685" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A686" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A687" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A688" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A689" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A690" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A691" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A692" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A693" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A694" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="695" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A695" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="696" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A696" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="697" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A697" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="698" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A698" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="699" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A699" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="700" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A700" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="701" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A701" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A702" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A703" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="704" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A704" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="705" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A705" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="706" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A706" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="707" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A707" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A708" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="709" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A709" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="710" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A710" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="711" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A711" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="712" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A712" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="713" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A713" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A714" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="715" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A715" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="716" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A716" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="717" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A717" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A718" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="719" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A719" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="720" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A720" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="721" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A721" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="722" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A722" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="723" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A723" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="724" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A724" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="725" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A725" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="726" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A726" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="727" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A727" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A728" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="729" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A729" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A730" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A731" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="732" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A732" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A733" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="734" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A734" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A735" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A736" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="737" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A737" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A738" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="739" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A739" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A740" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A741" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="742" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A742" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A743" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="744" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A744" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A745" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A746" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="747" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A747" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="748" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A748" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="749" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A749" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="750" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A750" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="751" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A751" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="752" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A752" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="753" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A753" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="754" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A754" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A755" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A756" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="757" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A757" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A758" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="759" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A759" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A760" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A761" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="762" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A762" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="763" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A763" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="764" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A764" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A765" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A766" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A767" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A768" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A769" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A770" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A771" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A772" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A773" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A774" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A775" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A776" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A777" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A778" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A779" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A780" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A781" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A782" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A783" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A784" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A785" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A786" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A787" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A788" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A789" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A790" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A791" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="792" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A792" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="793" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A793" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="794" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A794" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A795" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="796" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A796" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A797" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A798" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="799" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A799" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A800" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A801" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="802" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A802" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A803" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A804" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A805" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A806" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="807" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A807" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="808" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A808" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="809" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A809" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="810" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A810" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="811" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A811" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="812" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A812" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="813" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A813" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="814" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A814" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="815" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A815" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="816" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A816" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="817" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A817" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="818" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A818" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="819" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A819" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="820" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A820" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="821" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A821" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="822" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A822" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="823" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A823" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="824" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A824" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="825" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A825" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="826" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A826" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="827" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A827" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="828" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A828" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="829" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A829" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="830" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A830" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="831" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A831" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:AEZ832"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now reading in room capacities
</commit_message>
<xml_diff>
--- a/input/Data/TumOnline/Read15S.xlsx
+++ b/input/Data/TumOnline/Read15S.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="3" r:id="rId1"/>
-    <sheet name="Conflicts" sheetId="2" r:id="rId2"/>
+    <sheet name="Raum" sheetId="4" r:id="rId2"/>
+    <sheet name="Conflicts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +23,656 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="215">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Name_lang</t>
+  </si>
+  <si>
+    <t>Sitzplaetze</t>
+  </si>
+  <si>
+    <t>Klausurplaetze_eng</t>
+  </si>
+  <si>
+    <t>ID_Raum</t>
+  </si>
+  <si>
+    <t>ID_Gebaeude</t>
+  </si>
+  <si>
+    <t>Gebaeude</t>
+  </si>
+  <si>
+    <t>ID_Raumgruppe</t>
+  </si>
+  <si>
+    <t>ID_Campus</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>Audimax</t>
+  </si>
+  <si>
+    <t>0509.EG.980</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>HS_Innenstadt</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Innenstadt</t>
+  </si>
+  <si>
+    <t>Mensa_Garching</t>
+  </si>
+  <si>
+    <t>Mensa Garching</t>
+  </si>
+  <si>
+    <t>5302.EG.001</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>Mensa-Garching</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Garching</t>
+  </si>
+  <si>
+    <t>MW_2001</t>
+  </si>
+  <si>
+    <t>Rudolf-Diesel-Hörsaal Physik</t>
+  </si>
+  <si>
+    <t>5510.02.001</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>Carl-von-Linde-Hörsaal</t>
+  </si>
+  <si>
+    <t>0502.01.200</t>
+  </si>
+  <si>
+    <t>MW_0001</t>
+  </si>
+  <si>
+    <t>Gustav-Niemann-Hörsaal</t>
+  </si>
+  <si>
+    <t>5510.EG.001</t>
+  </si>
+  <si>
+    <t>MensaArcisSaalOst</t>
+  </si>
+  <si>
+    <t>Mensa Arcisstr. - großer Speisesaal</t>
+  </si>
+  <si>
+    <t>0206.01.103</t>
+  </si>
+  <si>
+    <t>Mensa</t>
+  </si>
+  <si>
+    <t>Mensa_Arcis</t>
+  </si>
+  <si>
+    <t>MI_HS_1</t>
+  </si>
+  <si>
+    <t>00.02.001 MI Hörsaal 1</t>
+  </si>
+  <si>
+    <t>5602.EG.001</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>MA-IN</t>
+  </si>
+  <si>
+    <t>MI_I1</t>
+  </si>
+  <si>
+    <t>101, Interims Hörsaal 1</t>
+  </si>
+  <si>
+    <t>5620.01.101</t>
+  </si>
+  <si>
+    <t>N1190</t>
+  </si>
+  <si>
+    <t>Hans Heinrich-Meinke Hörsaal</t>
+  </si>
+  <si>
+    <t>0101.01.190</t>
+  </si>
+  <si>
+    <t>Nord</t>
+  </si>
+  <si>
+    <t>MW_1801</t>
+  </si>
+  <si>
+    <t>Ernst-Schmidt-Hörsaal</t>
+  </si>
+  <si>
+    <t>5508.01.801</t>
+  </si>
+  <si>
+    <t>PH_HS_1</t>
+  </si>
+  <si>
+    <t>Hörsaal 1</t>
+  </si>
+  <si>
+    <t>5101.EG.501</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>MensaArcisSaalWest</t>
+  </si>
+  <si>
+    <t>Mensa Arcisstr. - kleiner Speisesaal</t>
+  </si>
+  <si>
+    <t>0206.01.103A</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>Friedrich von Thiersch Hörsaal</t>
+  </si>
+  <si>
+    <t>0503.02.300</t>
+  </si>
+  <si>
+    <t>2750</t>
+  </si>
+  <si>
+    <t>Karl Max von Bauernfeind Hörsaal</t>
+  </si>
+  <si>
+    <t>0507.03.750</t>
+  </si>
+  <si>
+    <t>N1179</t>
+  </si>
+  <si>
+    <t>Wilhelm-Nusselt-Hörsaal</t>
+  </si>
+  <si>
+    <t>0101.01.179</t>
+  </si>
+  <si>
+    <t>N1189</t>
+  </si>
+  <si>
+    <t>Hans-Piloty-Hörsaal</t>
+  </si>
+  <si>
+    <t>0101.01.189</t>
+  </si>
+  <si>
+    <t>CH_21010</t>
+  </si>
+  <si>
+    <t>Hans-Fischer-Hörsaal</t>
+  </si>
+  <si>
+    <t>5401.01.101K</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>MI_I2</t>
+  </si>
+  <si>
+    <t>102, Interims Hörsaal 2</t>
+  </si>
+  <si>
+    <t>5620.01.102</t>
+  </si>
+  <si>
+    <t>0360</t>
+  </si>
+  <si>
+    <t>Theodor-Fischer-Hörsaal</t>
+  </si>
+  <si>
+    <t>0503.EG.360</t>
+  </si>
+  <si>
+    <t>PR_35_HS_2</t>
+  </si>
+  <si>
+    <t>BC2 0.01.17</t>
+  </si>
+  <si>
+    <t>8102.EG.117</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>Hochbrück</t>
+  </si>
+  <si>
+    <t>Hochbrueck</t>
+  </si>
+  <si>
+    <t>02-81</t>
+  </si>
+  <si>
+    <t>Garching-Hochbrück</t>
+  </si>
+  <si>
+    <t>N1070</t>
+  </si>
+  <si>
+    <t>Lothar-Rohde-Hörsaal</t>
+  </si>
+  <si>
+    <t>0101.01.070</t>
+  </si>
+  <si>
+    <t>N1080</t>
+  </si>
+  <si>
+    <t>August-Föppl-Hörsaal</t>
+  </si>
+  <si>
+    <t>0101.01.080</t>
+  </si>
+  <si>
+    <t>MW_1450</t>
+  </si>
+  <si>
+    <t>Willy-Messerschmitt-Zeichensaal</t>
+  </si>
+  <si>
+    <t>5504.01.450</t>
+  </si>
+  <si>
+    <t>MW_Zeichnen</t>
+  </si>
+  <si>
+    <t>MW_1550</t>
+  </si>
+  <si>
+    <t>Georg-Kühne-Zeichensaal</t>
+  </si>
+  <si>
+    <t>5505.01.550</t>
+  </si>
+  <si>
+    <t>MW_1350</t>
+  </si>
+  <si>
+    <t>Ludwig-Burmester-Zeichensaal</t>
+  </si>
+  <si>
+    <t>5503.01.350</t>
+  </si>
+  <si>
+    <t>PH_HS_2</t>
+  </si>
+  <si>
+    <t>Hörsaal 2</t>
+  </si>
+  <si>
+    <t>5101.EG.502</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>Hörsaal ohne exp. Bühne</t>
+  </si>
+  <si>
+    <t>0501.01.100</t>
+  </si>
+  <si>
+    <t>1180</t>
+  </si>
+  <si>
+    <t>0501.01.180</t>
+  </si>
+  <si>
+    <t>0602</t>
+  </si>
+  <si>
+    <t>Theresianum, 0602</t>
+  </si>
+  <si>
+    <t>0506.EG.602</t>
+  </si>
+  <si>
+    <t>0606</t>
+  </si>
+  <si>
+    <t>Theresianum, 0606</t>
+  </si>
+  <si>
+    <t>0506.EG.606</t>
+  </si>
+  <si>
+    <t>MW_2050</t>
+  </si>
+  <si>
+    <t>Zeichen-/Hörsaal</t>
+  </si>
+  <si>
+    <t>5510.02.050</t>
+  </si>
+  <si>
+    <t>MW_350</t>
+  </si>
+  <si>
+    <t>Egbert-von-Hoyer-Hörsaal</t>
+  </si>
+  <si>
+    <t>5503.EG.350</t>
+  </si>
+  <si>
+    <t>MW_1050</t>
+  </si>
+  <si>
+    <t>Johann-Bauschinger-Zeichensaal</t>
+  </si>
+  <si>
+    <t>5510.01.050</t>
+  </si>
+  <si>
+    <t>0220</t>
+  </si>
+  <si>
+    <t>Hörsaal m. Exp.-Bühne</t>
+  </si>
+  <si>
+    <t>0502.EG.220</t>
+  </si>
+  <si>
+    <t>2770</t>
+  </si>
+  <si>
+    <t>Hörsaal</t>
+  </si>
+  <si>
+    <t>0507.02.770</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
+    <t>Übungsraum (ähnlich Zeichensaal)</t>
+  </si>
+  <si>
+    <t>0501.02.100</t>
+  </si>
+  <si>
+    <t>PR_35_HS_1</t>
+  </si>
+  <si>
+    <t>BC2 0.01.16</t>
+  </si>
+  <si>
+    <t>8102.EG.116</t>
+  </si>
+  <si>
+    <t>PR_37_3.5.06</t>
+  </si>
+  <si>
+    <t>Seminarraum 3</t>
+  </si>
+  <si>
+    <t>8102.03.506</t>
+  </si>
+  <si>
+    <t>PR_37_3.1.08</t>
+  </si>
+  <si>
+    <t>Seminarraum 1</t>
+  </si>
+  <si>
+    <t>8102.03.108</t>
+  </si>
+  <si>
+    <t>1260</t>
+  </si>
+  <si>
+    <t>Hörsaal o. Exp.-Bühne</t>
+  </si>
+  <si>
+    <t>0502.01.260</t>
+  </si>
+  <si>
+    <t>2370</t>
+  </si>
+  <si>
+    <t>HS 2370</t>
+  </si>
+  <si>
+    <t>0503.02.370</t>
+  </si>
+  <si>
+    <t>CH_22210</t>
+  </si>
+  <si>
+    <t>Ivar-Ugi-Hörsaal</t>
+  </si>
+  <si>
+    <t>5402.01.221K</t>
+  </si>
+  <si>
+    <t>CH_27402</t>
+  </si>
+  <si>
+    <t>Walter-Hieber-Hörsaal</t>
+  </si>
+  <si>
+    <t>5407.01.740B</t>
+  </si>
+  <si>
+    <t>MW_2450</t>
+  </si>
+  <si>
+    <t>Zeichensaal Galerie</t>
+  </si>
+  <si>
+    <t>5504.02.450</t>
+  </si>
+  <si>
+    <t>1402</t>
+  </si>
+  <si>
+    <t>0504.01.402</t>
+  </si>
+  <si>
+    <t>N1090</t>
+  </si>
+  <si>
+    <t>N 1090</t>
+  </si>
+  <si>
+    <t>0101.01.090</t>
+  </si>
+  <si>
+    <t>N1095</t>
+  </si>
+  <si>
+    <t>N 1095</t>
+  </si>
+  <si>
+    <t>0101.01.095</t>
+  </si>
+  <si>
+    <t>MI_HS_2</t>
+  </si>
+  <si>
+    <t>00.04.011 MI Hörsaal 2</t>
+  </si>
+  <si>
+    <t>5604.EG.011</t>
+  </si>
+  <si>
+    <t>MI_HS_3</t>
+  </si>
+  <si>
+    <t>00.06.011, MI Hörsaal 3</t>
+  </si>
+  <si>
+    <t>5606.EG.011</t>
+  </si>
+  <si>
+    <t>0601</t>
+  </si>
+  <si>
+    <t>Theresianum, 0601</t>
+  </si>
+  <si>
+    <t>0506.EG.601</t>
+  </si>
+  <si>
+    <t>MW_1250</t>
+  </si>
+  <si>
+    <t>5502.01.250</t>
+  </si>
+  <si>
+    <t>MW_0250</t>
+  </si>
+  <si>
+    <t>Ludwig-Prandtl-Hörsaal</t>
+  </si>
+  <si>
+    <t>5502.EG.250</t>
+  </si>
+  <si>
+    <t>0670</t>
+  </si>
+  <si>
+    <t>Theresianum, 0670ZG</t>
+  </si>
+  <si>
+    <t>0506.EG.670</t>
+  </si>
+  <si>
+    <t>1601</t>
+  </si>
+  <si>
+    <t>Theresianum, 1601, Hörsaal</t>
+  </si>
+  <si>
+    <t>0506.01.601</t>
+  </si>
+  <si>
+    <t>CH_26411</t>
+  </si>
+  <si>
+    <t>Emil-Erlenmeyer-Hörsaal</t>
+  </si>
+  <si>
+    <t>5406.01.641A</t>
+  </si>
+  <si>
+    <t>2760</t>
+  </si>
+  <si>
+    <t>Hörsaal (zu klein für PRKOORD)</t>
+  </si>
+  <si>
+    <t>0507.02.760</t>
+  </si>
+  <si>
+    <t>PH_HS_3</t>
+  </si>
+  <si>
+    <t>Hörsaal 3</t>
+  </si>
+  <si>
+    <t>5101.EG.503</t>
+  </si>
+  <si>
+    <t>CH_22209</t>
+  </si>
+  <si>
+    <t>Übungsraum</t>
+  </si>
+  <si>
+    <t>5402.01.220J</t>
+  </si>
+  <si>
+    <t>CH_26410</t>
+  </si>
+  <si>
+    <t>5406.01.641K</t>
+  </si>
+  <si>
+    <t>CH_27401</t>
+  </si>
+  <si>
+    <t>MW_2350</t>
+  </si>
+  <si>
+    <t>5503.02.350</t>
+  </si>
+  <si>
+    <t>MW_2550</t>
+  </si>
+  <si>
+    <t>5505.02.550</t>
+  </si>
+  <si>
+    <t>MW_0337</t>
+  </si>
+  <si>
+    <t>Seminarraum</t>
+  </si>
+  <si>
+    <t>5503.EG.337</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,8 +1007,8 @@
   <sheetPr codeName="Tabelle9"/>
   <dimension ref="A1:A831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A799" workbookViewId="0">
-      <selection activeCell="D828" sqref="D828"/>
+    <sheetView topLeftCell="A799" workbookViewId="0">
+      <selection activeCell="L821" sqref="L821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4526,6 +5177,2012 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>250</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>249</v>
+      </c>
+      <c r="D3">
+        <v>249</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>873</v>
+      </c>
+      <c r="D4">
+        <v>221</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>843</v>
+      </c>
+      <c r="D5">
+        <v>210</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>698</v>
+      </c>
+      <c r="D6">
+        <v>178</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>166</v>
+      </c>
+      <c r="D7">
+        <v>166</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>522</v>
+      </c>
+      <c r="D8">
+        <v>136</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>449</v>
+      </c>
+      <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>420</v>
+      </c>
+      <c r="D10">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11">
+        <v>401</v>
+      </c>
+      <c r="D11">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>395</v>
+      </c>
+      <c r="D12">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14">
+        <v>361</v>
+      </c>
+      <c r="D14">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15">
+        <v>319</v>
+      </c>
+      <c r="D15">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>308</v>
+      </c>
+      <c r="D16">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>308</v>
+      </c>
+      <c r="D17">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>319</v>
+      </c>
+      <c r="D18">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>286</v>
+      </c>
+      <c r="D19">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>209</v>
+      </c>
+      <c r="D21">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22">
+        <v>220</v>
+      </c>
+      <c r="D22">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23">
+        <v>220</v>
+      </c>
+      <c r="D23">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26">
+        <v>58</v>
+      </c>
+      <c r="D26">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27">
+        <v>194</v>
+      </c>
+      <c r="D27">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29">
+        <v>200</v>
+      </c>
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31">
+        <v>200</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33">
+        <v>180</v>
+      </c>
+      <c r="D33">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34">
+        <v>90</v>
+      </c>
+      <c r="D34">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35">
+        <v>175</v>
+      </c>
+      <c r="D35">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36">
+        <v>180</v>
+      </c>
+      <c r="D36">
+        <v>45</v>
+      </c>
+      <c r="E36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37">
+        <v>80</v>
+      </c>
+      <c r="D37">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38">
+        <v>77</v>
+      </c>
+      <c r="D38">
+        <v>39</v>
+      </c>
+      <c r="E38" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39">
+        <v>96</v>
+      </c>
+      <c r="D39">
+        <v>36</v>
+      </c>
+      <c r="E39" t="s">
+        <v>146</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" t="s">
+        <v>90</v>
+      </c>
+      <c r="I39" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40">
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40" t="s">
+        <v>90</v>
+      </c>
+      <c r="I40" t="s">
+        <v>91</v>
+      </c>
+      <c r="J40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41">
+        <v>143</v>
+      </c>
+      <c r="D41">
+        <v>35</v>
+      </c>
+      <c r="E41" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42">
+        <v>143</v>
+      </c>
+      <c r="D42">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43">
+        <v>122</v>
+      </c>
+      <c r="D43">
+        <v>32</v>
+      </c>
+      <c r="E43" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44">
+        <v>118</v>
+      </c>
+      <c r="D44">
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>164</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46">
+        <v>110</v>
+      </c>
+      <c r="D46">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47">
+        <v>110</v>
+      </c>
+      <c r="D47">
+        <v>27</v>
+      </c>
+      <c r="E47" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>50</v>
+      </c>
+      <c r="H47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48">
+        <v>110</v>
+      </c>
+      <c r="D48">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49">
+        <v>100</v>
+      </c>
+      <c r="D49">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50">
+        <v>100</v>
+      </c>
+      <c r="D50">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51">
+        <v>100</v>
+      </c>
+      <c r="D51">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>181</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52">
+        <v>88</v>
+      </c>
+      <c r="D52">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53">
+        <v>88</v>
+      </c>
+      <c r="D53">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>186</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54">
+        <v>100</v>
+      </c>
+      <c r="D54">
+        <v>25</v>
+      </c>
+      <c r="E54" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C55">
+        <v>100</v>
+      </c>
+      <c r="D55">
+        <v>25</v>
+      </c>
+      <c r="E55" t="s">
+        <v>192</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56">
+        <v>118</v>
+      </c>
+      <c r="D56">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>195</v>
+      </c>
+      <c r="F56" t="s">
+        <v>77</v>
+      </c>
+      <c r="G56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" t="s">
+        <v>197</v>
+      </c>
+      <c r="C57">
+        <v>96</v>
+      </c>
+      <c r="D57">
+        <v>24</v>
+      </c>
+      <c r="E57" t="s">
+        <v>198</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58" t="s">
+        <v>200</v>
+      </c>
+      <c r="C58">
+        <v>74</v>
+      </c>
+      <c r="D58">
+        <v>21</v>
+      </c>
+      <c r="E58" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" t="s">
+        <v>57</v>
+      </c>
+      <c r="G58" t="s">
+        <v>58</v>
+      </c>
+      <c r="H58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59">
+        <v>40</v>
+      </c>
+      <c r="D59">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
+        <v>204</v>
+      </c>
+      <c r="F59" t="s">
+        <v>77</v>
+      </c>
+      <c r="G59" t="s">
+        <v>78</v>
+      </c>
+      <c r="H59" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60">
+        <v>40</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="E60" t="s">
+        <v>206</v>
+      </c>
+      <c r="F60" t="s">
+        <v>77</v>
+      </c>
+      <c r="G60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H60" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>207</v>
+      </c>
+      <c r="B61" t="s">
+        <v>203</v>
+      </c>
+      <c r="C61">
+        <v>40</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>206</v>
+      </c>
+      <c r="F61" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" t="s">
+        <v>78</v>
+      </c>
+      <c r="H61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>208</v>
+      </c>
+      <c r="B62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>209</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>210</v>
+      </c>
+      <c r="B63" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>211</v>
+      </c>
+      <c r="F63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" t="s">
+        <v>21</v>
+      </c>
+      <c r="J63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" t="s">
+        <v>213</v>
+      </c>
+      <c r="C64">
+        <v>32</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>214</v>
+      </c>
+      <c r="F64" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:AEZ832"/>

</xml_diff>